<commit_message>
backend WEB. Udah konek sama database.
</commit_message>
<xml_diff>
--- a/WEB/alamin/assets/excel/Data Pegawai.xlsx
+++ b/WEB/alamin/assets/excel/Data Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -38,12 +38,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Samsul Huda</t>
-  </si>
-  <si>
-    <t>085234640114</t>
-  </si>
-  <si>
     <t>Antony Febriansyah Hartono</t>
   </si>
   <si>
@@ -62,52 +56,52 @@
     <t>085736333728</t>
   </si>
   <si>
+    <t>Mustofa Halim</t>
+  </si>
+  <si>
+    <t>081330493322</t>
+  </si>
+  <si>
+    <t>Dody Ahmad Kusuma Jaya</t>
+  </si>
+  <si>
+    <t>083854520015</t>
+  </si>
+  <si>
+    <t>Mokhammad Choirul Ikhsan</t>
+  </si>
+  <si>
+    <t>085749535400</t>
+  </si>
+  <si>
+    <t>Achmad Chadil Auwfar</t>
+  </si>
+  <si>
+    <t>08984119934</t>
+  </si>
+  <si>
+    <t>Rizal Ferdian</t>
+  </si>
+  <si>
+    <t>087777284179</t>
+  </si>
+  <si>
+    <t>Redika Angga Pratama</t>
+  </si>
+  <si>
+    <t>083834657395</t>
+  </si>
+  <si>
     <t>Tolkha Hasan</t>
   </si>
   <si>
     <t>081233072122</t>
   </si>
   <si>
-    <t>Mustofa Halim</t>
-  </si>
-  <si>
-    <t>081330493322</t>
-  </si>
-  <si>
-    <t>Dody Ahmad Kusuma Jaya</t>
-  </si>
-  <si>
-    <t>083854520015</t>
-  </si>
-  <si>
-    <t>Mokhammad Choirul Ikhsan</t>
-  </si>
-  <si>
-    <t>085749535400</t>
-  </si>
-  <si>
     <t>Wawan Dwi Prasetyo</t>
   </si>
   <si>
     <t>085745966707</t>
-  </si>
-  <si>
-    <t>Achmad Chadil Auwfar</t>
-  </si>
-  <si>
-    <t>08984119934</t>
-  </si>
-  <si>
-    <t>Rizal Ferdian</t>
-  </si>
-  <si>
-    <t>087777284179</t>
-  </si>
-  <si>
-    <t>Redika Angga Pratama</t>
-  </si>
-  <si>
-    <t>083834657395</t>
   </si>
 </sst>
 </file>
@@ -446,7 +440,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,7 +473,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -488,13 +482,13 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -502,7 +496,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -525,7 +519,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -540,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -548,7 +542,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -563,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -571,7 +565,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -586,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -594,7 +588,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -603,13 +597,13 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -617,7 +611,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -626,13 +620,13 @@
         <v>20</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -640,7 +634,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -649,13 +643,13 @@
         <v>22</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>3</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -663,7 +657,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -672,13 +666,13 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -686,7 +680,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -701,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -709,7 +703,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
@@ -718,38 +712,15 @@
         <v>28</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13">
         <v>1</v>
       </c>
     </row>

</xml_diff>